<commit_message>
REsolve issue with temp FEDs
</commit_message>
<xml_diff>
--- a/Tables/FED_Table_020617.xlsx
+++ b/Tables/FED_Table_020617.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13350"/>
   </bookViews>
   <sheets>
-    <sheet name="FED_Table_020617" sheetId="1" r:id="rId1"/>
+    <sheet name="FED_Table" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
   <si>
     <t>Experiment</t>
   </si>
@@ -72,34 +72,34 @@
     <t>Transitional</t>
   </si>
   <si>
-    <t>N/A 0.012</t>
-  </si>
-  <si>
-    <t>N/A 0.035</t>
-  </si>
-  <si>
-    <t>N/A 0.015</t>
-  </si>
-  <si>
-    <t>N/A 0.326</t>
+    <t>N/A (0.012)</t>
+  </si>
+  <si>
+    <t>N/A (0.035)</t>
+  </si>
+  <si>
+    <t>N/A (0.015)</t>
+  </si>
+  <si>
+    <t>N/A (0.326)</t>
   </si>
   <si>
     <t>No Data</t>
   </si>
   <si>
-    <t>N/A 0.019</t>
-  </si>
-  <si>
-    <t>N/A 0.009</t>
-  </si>
-  <si>
-    <t>N/A 0.008</t>
-  </si>
-  <si>
-    <t>N/A 0.293</t>
-  </si>
-  <si>
-    <t>N/A 0.033</t>
+    <t>N/A (0.019)</t>
+  </si>
+  <si>
+    <t>N/A (0.009)</t>
+  </si>
+  <si>
+    <t>N/A (0.008)</t>
+  </si>
+  <si>
+    <t>N/A (0.293)</t>
+  </si>
+  <si>
+    <t>N/A (0.033)</t>
   </si>
   <si>
     <t>Experiment_02</t>
@@ -108,64 +108,64 @@
     <t>Interior</t>
   </si>
   <si>
-    <t>N/A 0.251</t>
-  </si>
-  <si>
-    <t>N/A 0.038</t>
-  </si>
-  <si>
-    <t>N/A 0.089</t>
-  </si>
-  <si>
-    <t>N/A 0.153</t>
-  </si>
-  <si>
-    <t>N/A 0.037</t>
-  </si>
-  <si>
-    <t>N/A 0.022</t>
-  </si>
-  <si>
-    <t>N/A 0.066</t>
+    <t>N/A (0.251)</t>
+  </si>
+  <si>
+    <t>N/A (0.038)</t>
+  </si>
+  <si>
+    <t>N/A (0.089)</t>
+  </si>
+  <si>
+    <t>N/A (0.153)</t>
+  </si>
+  <si>
+    <t>N/A (0.037)</t>
+  </si>
+  <si>
+    <t>N/A (0.022)</t>
+  </si>
+  <si>
+    <t>N/A (0.066)</t>
   </si>
   <si>
     <t>Experiment_03</t>
   </si>
   <si>
-    <t>N/A 0.362</t>
+    <t>N/A (0.362)</t>
   </si>
   <si>
     <t>Sensor Malfunction at 1895.0</t>
   </si>
   <si>
-    <t>N/A 0.041</t>
-  </si>
-  <si>
-    <t>N/A 0.027</t>
-  </si>
-  <si>
-    <t>N/A 0.017</t>
-  </si>
-  <si>
-    <t>N/A 0.321</t>
-  </si>
-  <si>
-    <t>N/A 0.051</t>
+    <t>N/A (0.041)</t>
+  </si>
+  <si>
+    <t>N/A (0.027)</t>
+  </si>
+  <si>
+    <t>N/A (0.017)</t>
+  </si>
+  <si>
+    <t>N/A (0.321)</t>
+  </si>
+  <si>
+    <t>N/A (0.051)</t>
   </si>
   <si>
     <t>Experiment_04</t>
   </si>
   <si>
-    <t>N/A 0.274</t>
-  </si>
-  <si>
-    <t>N/A 0.016</t>
-  </si>
-  <si>
-    <t>N/A 0.209</t>
-  </si>
-  <si>
-    <t>N/A 0.043</t>
+    <t>N/A (0.274)</t>
+  </si>
+  <si>
+    <t>N/A (0.016)</t>
+  </si>
+  <si>
+    <t>N/A (0.209)</t>
+  </si>
+  <si>
+    <t>N/A (0.043)</t>
   </si>
   <si>
     <t>Sensor Malfunction at 1.0</t>
@@ -174,163 +174,145 @@
     <t>Sensor Malfunction at 1609.0</t>
   </si>
   <si>
-    <t>N/A 0.02</t>
-  </si>
-  <si>
-    <t>N/A 0.028</t>
-  </si>
-  <si>
-    <t>N/A 0.332</t>
+    <t>N/A (0.02)</t>
+  </si>
+  <si>
+    <t>N/A (0.028)</t>
   </si>
   <si>
     <t>Experiment_05</t>
   </si>
   <si>
-    <t>N/A 0.762</t>
+    <t>N/A (0.762)</t>
   </si>
   <si>
     <t>Sensor Malfunction at 138.0</t>
   </si>
   <si>
-    <t>N/A 0.286</t>
-  </si>
-  <si>
-    <t>N/A 0.072</t>
-  </si>
-  <si>
-    <t>N/A 0.034</t>
-  </si>
-  <si>
-    <t>N/A 0.357</t>
-  </si>
-  <si>
-    <t>N/A 0.074</t>
+    <t>N/A (0.286)</t>
+  </si>
+  <si>
+    <t>N/A (0.072)</t>
+  </si>
+  <si>
+    <t>N/A (0.034)</t>
+  </si>
+  <si>
+    <t>N/A (0.074)</t>
   </si>
   <si>
     <t>Experiment_06</t>
   </si>
   <si>
-    <t>N/A 0.717</t>
-  </si>
-  <si>
-    <t>N/A 0.283</t>
-  </si>
-  <si>
-    <t>N/A 0.024</t>
-  </si>
-  <si>
-    <t>N/A 0.092</t>
-  </si>
-  <si>
-    <t>N/A 0.023</t>
+    <t>N/A (0.717)</t>
+  </si>
+  <si>
+    <t>N/A (0.283)</t>
+  </si>
+  <si>
+    <t>N/A (0.024)</t>
   </si>
   <si>
     <t>Experiment_07</t>
   </si>
   <si>
-    <t>N/A 0.572</t>
-  </si>
-  <si>
-    <t>N/A 0.582</t>
-  </si>
-  <si>
-    <t>N/A 0.258</t>
-  </si>
-  <si>
-    <t>N/A 0.026</t>
-  </si>
-  <si>
-    <t>N/A 0.018</t>
-  </si>
-  <si>
-    <t>N/A 0.014</t>
-  </si>
-  <si>
-    <t>N/A 0.452</t>
-  </si>
-  <si>
-    <t>N/A 0.021</t>
+    <t>N/A (0.572)</t>
+  </si>
+  <si>
+    <t>N/A (0.582)</t>
+  </si>
+  <si>
+    <t>N/A (0.258)</t>
+  </si>
+  <si>
+    <t>N/A (0.026)</t>
+  </si>
+  <si>
+    <t>N/A (0.018)</t>
+  </si>
+  <si>
+    <t>N/A (0.014)</t>
+  </si>
+  <si>
+    <t>N/A (0.452)</t>
   </si>
   <si>
     <t>Experiment_08</t>
   </si>
   <si>
-    <t>N/A 0.414</t>
-  </si>
-  <si>
-    <t>N/A 0.351</t>
-  </si>
-  <si>
-    <t>N/A 0.124</t>
-  </si>
-  <si>
-    <t>N/A 0.039</t>
+    <t>N/A (0.414)</t>
+  </si>
+  <si>
+    <t>N/A (0.351)</t>
+  </si>
+  <si>
+    <t>N/A (0.039)</t>
   </si>
   <si>
     <t>Experiment_09</t>
   </si>
   <si>
-    <t>N/A 0.211</t>
-  </si>
-  <si>
-    <t>N/A 0.719</t>
-  </si>
-  <si>
-    <t>N/A 0.133</t>
-  </si>
-  <si>
-    <t>N/A 0.34</t>
+    <t>N/A (0.211)</t>
+  </si>
+  <si>
+    <t>N/A (0.719)</t>
+  </si>
+  <si>
+    <t>N/A (0.133)</t>
+  </si>
+  <si>
+    <t>N/A (0.34)</t>
   </si>
   <si>
     <t>Experiment_10</t>
   </si>
   <si>
-    <t>N/A 0.059</t>
-  </si>
-  <si>
-    <t>N/A 0.001</t>
-  </si>
-  <si>
-    <t>N/A 0.106</t>
-  </si>
-  <si>
-    <t>N/A 0.032</t>
-  </si>
-  <si>
-    <t>N/A 0.031</t>
+    <t>N/A (0.059)</t>
+  </si>
+  <si>
+    <t>N/A (0.001)</t>
+  </si>
+  <si>
+    <t>N/A (0.106)</t>
+  </si>
+  <si>
+    <t>N/A (0.032)</t>
+  </si>
+  <si>
+    <t>N/A (0.031)</t>
+  </si>
+  <si>
+    <t>N/A (0.332)</t>
   </si>
   <si>
     <t>Experiment_11</t>
   </si>
   <si>
-    <t>N/A -0.001</t>
-  </si>
-  <si>
-    <t>N/A 0.849</t>
-  </si>
-  <si>
-    <t>N/A 0.108</t>
-  </si>
-  <si>
-    <t>N/A 0.036</t>
-  </si>
-  <si>
-    <t>N/A 0.546</t>
+    <t>N/A (-0.001)</t>
+  </si>
+  <si>
+    <t>N/A (0.849)</t>
+  </si>
+  <si>
+    <t>N/A (0.108)</t>
+  </si>
+  <si>
+    <t>N/A (0.036)</t>
   </si>
   <si>
     <t>Experiment_12</t>
   </si>
   <si>
-    <t>N/A 0.003</t>
-  </si>
-  <si>
-    <t>N/A 0.064</t>
-  </si>
-  <si>
-    <t>N/A 0.04</t>
-  </si>
-  <si>
-    <t>N/A 0.672</t>
+    <t>N/A (0.003)</t>
+  </si>
+  <si>
+    <t>N/A (0.064)</t>
+  </si>
+  <si>
+    <t>N/A (0.04)</t>
+  </si>
+  <si>
+    <t>N/A (0.672)</t>
   </si>
 </sst>
 </file>
@@ -654,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -769,6 +751,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -814,8 +811,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1173,635 +1173,627 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>854</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>300</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2137</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>344</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>466</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1984</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>442</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>984</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>513</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>345</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>2062</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>300</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O5">
-        <v>1035</v>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2148</v>
+      </c>
+      <c r="D6" s="1">
+        <v>465</v>
+      </c>
+      <c r="E6" s="1">
+        <v>927</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="1">
+        <v>813</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1">
+        <v>341</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2063</v>
+      </c>
+      <c r="D7" s="1">
+        <v>623</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="1">
+        <v>972</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1277</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="1">
+        <v>344</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6">
-        <v>2148</v>
-      </c>
-      <c r="D6">
-        <v>465</v>
-      </c>
-      <c r="E6">
-        <v>927</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6">
-        <v>813</v>
-      </c>
-      <c r="H6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6">
-        <v>341</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="C8" s="1">
+        <v>1931</v>
+      </c>
+      <c r="D8" s="1">
+        <v>419</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="1">
+        <v>474</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="1">
+        <v>346</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2063</v>
+      </c>
+      <c r="D9" s="1">
+        <v>409</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1068</v>
+      </c>
+      <c r="G9" s="1">
+        <v>876</v>
+      </c>
+      <c r="H9" s="1">
+        <v>132</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="1">
+        <v>262</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1980</v>
+      </c>
+      <c r="D10" s="1">
+        <v>408</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1">
+        <v>476</v>
+      </c>
+      <c r="H10" s="1">
+        <v>50</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="1">
+        <v>225</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1811</v>
+      </c>
+      <c r="D11" s="1">
+        <v>444</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="1">
+        <v>976</v>
+      </c>
+      <c r="H11" s="1">
+        <v>160</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="1">
+        <v>365</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1831</v>
+      </c>
+      <c r="D12" s="1">
+        <v>371</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="1">
+        <v>456</v>
+      </c>
+      <c r="H12" s="1">
+        <v>62</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="1">
+        <v>315</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L6" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="M12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6" t="s">
-        <v>61</v>
+      <c r="N12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>2063</v>
-      </c>
-      <c r="D7">
-        <v>623</v>
-      </c>
-      <c r="E7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7">
-        <v>972</v>
-      </c>
-      <c r="H7">
-        <v>1277</v>
-      </c>
-      <c r="I7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7">
-        <v>344</v>
-      </c>
-      <c r="K7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" t="s">
-        <v>65</v>
-      </c>
-      <c r="M7" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" t="s">
-        <v>66</v>
-      </c>
-      <c r="O7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8">
-        <v>1931</v>
-      </c>
-      <c r="D8">
-        <v>419</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8">
-        <v>474</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="C13" s="1">
+        <v>1854</v>
+      </c>
+      <c r="D13" s="1">
+        <v>442</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="1">
+        <v>635</v>
+      </c>
+      <c r="H13" s="1">
+        <v>184</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" s="1">
+        <v>373</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8">
-        <v>346</v>
-      </c>
-      <c r="K8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" t="s">
-        <v>73</v>
-      </c>
-      <c r="M8" t="s">
-        <v>74</v>
-      </c>
-      <c r="N8" t="s">
-        <v>75</v>
-      </c>
-      <c r="O8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>2063</v>
-      </c>
-      <c r="D9">
-        <v>409</v>
-      </c>
-      <c r="E9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9">
-        <v>1068</v>
-      </c>
-      <c r="G9">
-        <v>876</v>
-      </c>
-      <c r="H9">
-        <v>132</v>
-      </c>
-      <c r="I9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9">
-        <v>262</v>
-      </c>
-      <c r="K9" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" t="s">
-        <v>80</v>
-      </c>
-      <c r="O9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10">
-        <v>1980</v>
-      </c>
-      <c r="D10">
-        <v>408</v>
-      </c>
-      <c r="E10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10">
-        <v>476</v>
-      </c>
-      <c r="H10">
-        <v>50</v>
-      </c>
-      <c r="I10" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10">
-        <v>225</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
-        <v>72</v>
-      </c>
-      <c r="M10" t="s">
-        <v>73</v>
-      </c>
-      <c r="N10" t="s">
-        <v>86</v>
-      </c>
-      <c r="O10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>1811</v>
-      </c>
-      <c r="D11">
-        <v>444</v>
-      </c>
-      <c r="E11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11">
-        <v>976</v>
-      </c>
-      <c r="H11">
-        <v>160</v>
-      </c>
-      <c r="I11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11">
-        <v>365</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="N13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="L11" t="s">
-        <v>92</v>
-      </c>
-      <c r="M11" t="s">
-        <v>72</v>
-      </c>
-      <c r="N11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>1831</v>
-      </c>
-      <c r="D12">
-        <v>371</v>
-      </c>
-      <c r="E12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12">
-        <v>456</v>
-      </c>
-      <c r="H12">
-        <v>62</v>
-      </c>
-      <c r="I12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12">
-        <v>315</v>
-      </c>
-      <c r="K12" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" t="s">
-        <v>59</v>
-      </c>
-      <c r="M12" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12" t="s">
-        <v>98</v>
-      </c>
-      <c r="O12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
-        <v>1854</v>
-      </c>
-      <c r="D13">
-        <v>442</v>
-      </c>
-      <c r="E13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13">
-        <v>635</v>
-      </c>
-      <c r="H13">
-        <v>184</v>
-      </c>
-      <c r="I13" t="s">
-        <v>101</v>
-      </c>
-      <c r="J13">
-        <v>373</v>
-      </c>
-      <c r="K13" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" t="s">
-        <v>102</v>
-      </c>
-      <c r="M13" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" t="s">
-        <v>103</v>
-      </c>
-      <c r="O13" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>